<commit_message>
redid normal day shifts, added corresponding preferences in doctors input
</commit_message>
<xml_diff>
--- a/example/doctors.xlsx
+++ b/example/doctors.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
   <si>
     <t xml:space="preserve">ward</t>
   </si>
@@ -40,7 +40,13 @@
     <t xml:space="preserve">number_of_shifts_factor</t>
   </si>
   <si>
-    <t xml:space="preserve">long_day_hours</t>
+    <t xml:space="preserve">min_day_hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_day_hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preferred_day_hours</t>
   </si>
   <si>
     <t xml:space="preserve">fill_all_days</t>
@@ -64,6 +70,9 @@
     <t xml:space="preserve">no</t>
   </si>
   <si>
+    <t xml:space="preserve">min</t>
+  </si>
+  <si>
     <t xml:space="preserve">Crusher</t>
   </si>
   <si>
@@ -74,6 +83,9 @@
   </si>
   <si>
     <t xml:space="preserve">12_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max</t>
   </si>
   <si>
     <t xml:space="preserve">Bashir</t>
@@ -194,7 +206,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -205,15 +217,17 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.73"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.73"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -247,13 +261,19 @@
       <c r="K1" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="L1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>40</v>
@@ -262,10 +282,10 @@
         <v>44</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>1</v>
@@ -273,22 +293,28 @@
       <c r="H2" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="I2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" s="0" t="n">
+      <c r="I2" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>40</v>
@@ -297,33 +323,39 @@
         <v>44</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>40</v>
@@ -332,33 +364,39 @@
         <v>44</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I4" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="I4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="0" t="n">
+      <c r="J4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>40</v>
@@ -367,33 +405,39 @@
         <v>44</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>40</v>
@@ -402,33 +446,39 @@
         <v>44</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I6" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="I6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" s="0" t="n">
+      <c r="J6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>40</v>
@@ -437,33 +487,39 @@
         <v>44</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>40</v>
@@ -472,33 +528,39 @@
         <v>44</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="I8" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" s="0" t="n">
+      <c r="J8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>40</v>
@@ -507,33 +569,39 @@
         <v>44</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>40</v>
@@ -542,24 +610,30 @@
         <v>44</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G10" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H10" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I10" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="I10" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" s="0" t="n">
+      <c r="J10" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="0" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added keep_weekends_apart variable, split example script in 2 parts
</commit_message>
<xml_diff>
--- a/example/doctors.xlsx
+++ b/example/doctors.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="31">
   <si>
     <t xml:space="preserve">ward</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">friday_sunday</t>
   </si>
   <si>
+    <t xml:space="preserve">keep_weekends_apart</t>
+  </si>
+  <si>
     <t xml:space="preserve">number_of_shifts_factor</t>
   </si>
   <si>
@@ -70,28 +73,28 @@
     <t xml:space="preserve">no</t>
   </si>
   <si>
+    <t xml:space="preserve">max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crusher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pulaski</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bashir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4_3</t>
+  </si>
+  <si>
     <t xml:space="preserve">min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crusher</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pulaski</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bashir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4_3</t>
   </si>
   <si>
     <t xml:space="preserve">TheDoctor</t>
@@ -206,7 +209,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -220,14 +223,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.73"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.73"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -267,13 +271,16 @@
       <c r="M1" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="N1" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>40</v>
@@ -282,80 +289,86 @@
         <v>44</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J2" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="J2" s="0" t="s">
-        <v>16</v>
-      </c>
       <c r="K2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="0" t="n">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="M2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="K3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>44</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" s="0" t="n">
-        <v>0</v>
+      <c r="L3" s="0" t="s">
+        <v>15</v>
       </c>
       <c r="M3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>40</v>
@@ -364,30 +377,33 @@
         <v>44</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J4" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="J4" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="K4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" s="0" t="n">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="M4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -405,36 +421,39 @@
         <v>44</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J5" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="J5" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="K5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" s="0" t="n">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="M5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>23</v>
@@ -446,39 +465,42 @@
         <v>44</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H6" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J6" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="J6" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="K6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6" s="0" t="n">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="M6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>40</v>
@@ -487,39 +509,42 @@
         <v>44</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J7" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="J7" s="0" t="s">
-        <v>16</v>
-      </c>
       <c r="K7" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="L7" s="0" t="n">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="M7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>40</v>
@@ -528,39 +553,42 @@
         <v>44</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I8" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="J8" s="0" t="s">
-        <v>16</v>
-      </c>
       <c r="K8" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="L8" s="0" t="n">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="M8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>40</v>
@@ -569,39 +597,42 @@
         <v>44</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I9" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="J9" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="K9" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="L9" s="0" t="n">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="M9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>40</v>
@@ -610,30 +641,33 @@
         <v>44</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I10" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J10" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="J10" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="K10" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="L10" s="0" t="n">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>15</v>
       </c>
       <c r="M10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" s="0" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed hours/weekhours variables, added weeding out of nonsensical/conflicting requests
</commit_message>
<xml_diff>
--- a/example/doctors.xlsx
+++ b/example/doctors.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">ward</t>
   </si>
   <si>
-    <t xml:space="preserve">weekhours</t>
+    <t xml:space="preserve">weekhours_min</t>
   </si>
   <si>
     <t xml:space="preserve">weekhours_max</t>
@@ -219,7 +219,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.31"/>

</xml_diff>

<commit_message>
minor changes, and updated Anleitung
</commit_message>
<xml_diff>
--- a/example/doctors.xlsx
+++ b/example/doctors.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="29">
   <si>
     <t xml:space="preserve">ward</t>
   </si>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">McCoy</t>
   </si>
   <si>
-    <t xml:space="preserve">4_2</t>
+    <t xml:space="preserve">4_2_4_1</t>
   </si>
   <si>
     <t xml:space="preserve">yes</t>
@@ -79,15 +79,9 @@
     <t xml:space="preserve">Crusher</t>
   </si>
   <si>
-    <t xml:space="preserve">4_1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pulaski</t>
   </si>
   <si>
-    <t xml:space="preserve">12_2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bashir</t>
   </si>
   <si>
@@ -103,6 +97,9 @@
     <t xml:space="preserve">Phlox</t>
   </si>
   <si>
+    <t xml:space="preserve">12_2_6_3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Culber</t>
   </si>
   <si>
@@ -110,9 +107,6 @@
   </si>
   <si>
     <t xml:space="preserve">Cottle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6_3</t>
   </si>
 </sst>
 </file>
@@ -218,8 +212,8 @@
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.31"/>
@@ -324,7 +318,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>40</v>
@@ -365,10 +359,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>40</v>
@@ -380,7 +374,7 @@
         <v>15</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>5</v>
@@ -409,10 +403,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>40</v>
@@ -439,7 +433,7 @@
         <v>8</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L5" s="0" t="s">
         <v>16</v>
@@ -453,10 +447,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>40</v>
@@ -497,10 +491,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>40</v>
@@ -541,10 +535,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>40</v>
@@ -556,7 +550,7 @@
         <v>15</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>5</v>
@@ -585,10 +579,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>40</v>
@@ -629,10 +623,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>40</v>
@@ -659,7 +653,7 @@
         <v>7</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L10" s="0" t="s">
         <v>15</v>

</xml_diff>